<commit_message>
Changed column from "deprecated?" to "state"
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Participant identifier schemes v8.0.xlsx
+++ b/work-in-progress/Peppol Code Lists - Participant identifier schemes v8.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\peppol-edec-codelists\work-in-progress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCF0193-95DE-4AD6-9147-86289DF6BED3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6260DE6A-A478-46DA-9D87-E49F754550C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,38 +19,45 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Participant Identifier Scheme'!$A$1:$M$89</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author/>
+    <author>Philip Helger</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{6C21FA92-6BAE-49C0-9BE3-F0974AD124A5}">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Philip Helger:
-</t>
+          <t>Philip Helger:</t>
         </r>
         <r>
           <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
             <charset val="1"/>
           </rPr>
-          <t>ISO6523 identifier</t>
+          <t xml:space="preserve">
+ISO6523 identifier</t>
         </r>
       </text>
     </comment>
@@ -59,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="505">
   <si>
     <t>Scheme ID</t>
   </si>
@@ -77,12 +84,6 @@
   </si>
   <si>
     <t>Since</t>
-  </si>
-  <si>
-    <t>Deprecated</t>
-  </si>
-  <si>
-    <t>Deprecated since</t>
   </si>
   <si>
     <t>Structure of code</t>
@@ -1205,14 +1206,7 @@
     <t>Koordinierungsstelle für IT-Standards (KoSIT)</t>
   </si>
   <si>
-    <t>Up to 44 alphanumeric characters
-Format: “Up to 12 numeric characters – up to 30 alphanumeric characters – 2 numeric characters”</t>
-  </si>
-  <si>
     <t>Whole string</t>
-  </si>
-  <si>
-    <t>Each part is somehow optional</t>
   </si>
   <si>
     <t>1) Number of characters: 9 characters ("SIREN") 14 " 9+5 ("SIRET"), The 9 character number designates an organization, The 14 character number designates a specific establishment of the organization designated by the first 9 characters.
@@ -1612,9 +1606,6 @@
 No checkdigit</t>
   </si>
   <si>
-    <t>RegEx: [0-9]{0,12}(\-[0-9a-zA-Z]{0,30}(\-[0-9]{2}))</t>
-  </si>
-  <si>
     <t>RegEx: [1-9][0-9]{7}
 Check digit: mod11 (weights, 2, 7, 6, 5, 4, 3, 2, 1)</t>
   </si>
@@ -1781,6 +1772,28 @@
   </si>
   <si>
     <t>IT:IVA</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>deprecated</t>
+  </si>
+  <si>
+    <t>Deprecation version</t>
+  </si>
+  <si>
+    <t>Up to 46 alphanumeric characters
+Format: &lt;Up to 12 numeric characters&gt;"-"&lt;up to 30 alphanumeric characters&gt;"–"&lt;2 numeric characters&gt;</t>
+  </si>
+  <si>
+    <t>The fine grained part is optional</t>
+  </si>
+  <si>
+    <t>RegEx: [0-9]{2,12}(\-[0-9A-Z]{0,30})?\-[0-9]{2}</t>
   </si>
 </sst>
 </file>
@@ -1816,18 +1829,16 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -2191,6 +2202,60 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>866775</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1333500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C5391D-7B43-478A-ACB6-7AD0D8EF75E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9734550" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2518,25 +2583,25 @@
   <dimension ref="A1:AMM89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="62.28515625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="62.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="45.140625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="30.5703125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="30.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="30.5703125" style="13" customWidth="1"/>
     <col min="13" max="13" width="24.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="1026" width="14.140625" style="1" customWidth="1"/>
@@ -2563,1032 +2628,1004 @@
         <v>5</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>433</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>437</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>389</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>438</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>374</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="K3" s="2" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>375</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>29</v>
-      </c>
       <c r="K4" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="K5" s="2" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="195" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="210" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="G10" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="G11" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="J11" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="240" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="G14" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="J14" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G14" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>83</v>
-      </c>
       <c r="K14" s="2" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>443</v>
+      </c>
+      <c r="M15" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G15" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>342</v>
-      </c>
-      <c r="L15" s="13" t="s">
-        <v>447</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="E16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G16" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="G16" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="L16" s="13" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="M16" s="12"/>
     </row>
     <row r="17" spans="1:1027" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G17" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="G17" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="18" spans="1:1027" ht="225" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G18" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="19" spans="1:1027" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="F19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="I19" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G19" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>103</v>
-      </c>
       <c r="J19" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="L19" s="13" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="20" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="G20" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="I20" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G20" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>110</v>
-      </c>
       <c r="J20" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L20" s="13" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="21" spans="1:1027" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G21" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="L21" s="13" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="22" spans="1:1027" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G22" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="L22" s="13" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="23" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="I23" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="J23" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G23" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>353</v>
-      </c>
       <c r="L23" s="13" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="24" spans="1:1027" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="F24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="J24" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G24" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="8" t="s">
-        <v>387</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>357</v>
-      </c>
       <c r="L24" s="13" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="25" spans="1:1027" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="F25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="I25" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G25" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>126</v>
-      </c>
       <c r="J25" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="26" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="G26" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="I26" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="G26" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I26" s="8" t="s">
-        <v>364</v>
-      </c>
       <c r="J26" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="15" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="AMM26" s="1"/>
     </row>
     <row r="27" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="F27" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>502</v>
+      </c>
+      <c r="J27" s="8" t="s">
         <v>368</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="G27" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>371</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="15" t="s">
-        <v>459</v>
+        <v>504</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>372</v>
+        <v>503</v>
       </c>
       <c r="AMM27" s="1"/>
     </row>
     <row r="28" spans="1:1027" ht="165" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="J28" s="8" t="s">
         <v>430</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="G28" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>471</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>434</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="13" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="AMM28" s="1"/>
     </row>
     <row r="29" spans="1:1027" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>475</v>
-      </c>
-      <c r="G29" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>470</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="8" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K29" s="15" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="L29" s="13" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="M29" s="12"/>
       <c r="N29" s="12"/>
@@ -4608,34 +4645,33 @@
     </row>
     <row r="30" spans="1:1027" ht="255" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>475</v>
-      </c>
-      <c r="G30" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>470</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="8" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="K30" s="15"/>
       <c r="L30" s="13" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="M30" s="12"/>
       <c r="N30" s="12"/>
@@ -5655,34 +5691,33 @@
     </row>
     <row r="31" spans="1:1027" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="B31" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="12" t="s">
         <v>480</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>485</v>
-      </c>
       <c r="E31" s="12" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>475</v>
-      </c>
-      <c r="G31" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>470</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="H31" s="12"/>
       <c r="I31" s="8" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="K31" s="15"/>
       <c r="L31" s="13" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="M31" s="12"/>
       <c r="N31" s="12"/>
@@ -6702,37 +6737,36 @@
     </row>
     <row r="32" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>484</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>487</v>
+      </c>
+      <c r="E32" s="12" t="s">
         <v>488</v>
       </c>
-      <c r="B32" s="12" t="s">
-        <v>489</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>492</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>493</v>
-      </c>
       <c r="F32" s="15" t="s">
-        <v>475</v>
-      </c>
-      <c r="G32" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>470</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="H32" s="12"/>
       <c r="I32" s="8" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="K32" s="15"/>
       <c r="L32" s="13" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="M32" s="12"/>
       <c r="N32" s="12"/>
@@ -7752,37 +7786,36 @@
     </row>
     <row r="33" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>475</v>
-      </c>
-      <c r="G33" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>470</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="H33" s="12"/>
       <c r="I33" s="8" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="K33" s="15"/>
       <c r="L33" s="13" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="M33" s="12"/>
       <c r="N33" s="12"/>
@@ -8802,1397 +8835,1341 @@
     </row>
     <row r="34" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="E34" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="I34" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>130</v>
-      </c>
       <c r="J34" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="35" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="E35" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="L35" s="13" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
     </row>
     <row r="36" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="E36" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="K36" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="L36" s="13" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
     </row>
     <row r="37" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="E37" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="38" spans="1:1027" ht="105" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="F38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="K38" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G38" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="L38" s="13" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
     <row r="39" spans="1:1027" ht="285" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="E39" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G39" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="L39" s="13" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="40" spans="1:1027" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="F40" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G40" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L40" s="13" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="41" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G41" s="7" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="K41" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L41" s="13" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="42" spans="1:1027" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="F42" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G42" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="L42" s="13" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
     </row>
     <row r="43" spans="1:1027" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="E43" s="9"/>
       <c r="F43" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G43" s="7" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>500</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L43" s="13" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="M43" s="12" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
     </row>
     <row r="44" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="E44" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G44" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="45" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D45" s="1" t="s">
+      <c r="F45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="K45" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G45" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="E46" s="9"/>
       <c r="F46" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G46" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="L46" s="13" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="47" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D47" s="1" t="s">
+      <c r="F47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="H47" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G47" s="7" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="48" spans="1:1027" ht="105" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="J48" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="L48" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="M48" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G48" s="7" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I48" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="J48" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="L48" s="13" t="s">
-        <v>454</v>
-      </c>
-      <c r="M48" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="G49" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="G49" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="E50" s="9"/>
       <c r="F50" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G50" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>177</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="D51" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G51" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>177</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G52" s="7" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <v>151</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>500</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="E53" s="9"/>
       <c r="F53" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G53" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="E54" s="9"/>
       <c r="F54" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G54" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="E55" s="9"/>
       <c r="F55" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G55" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="E56" s="9"/>
       <c r="F56" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G56" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="E57" s="9"/>
       <c r="F57" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G57" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="E58" s="9"/>
       <c r="F58" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G58" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>222</v>
-      </c>
       <c r="F59" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G59" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="E60" s="9"/>
       <c r="F60" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G60" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="E61" s="9"/>
       <c r="F61" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G61" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="E62" s="9"/>
       <c r="F62" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G62" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="E63" s="9"/>
       <c r="F63" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G63" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="E64" s="9"/>
       <c r="F64" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G64" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G64" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>245</v>
       </c>
       <c r="E65" s="9"/>
       <c r="F65" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G65" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>249</v>
       </c>
       <c r="E66" s="9"/>
       <c r="F66" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G66" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="E67" s="9"/>
       <c r="F67" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G67" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>256</v>
       </c>
       <c r="E68" s="9"/>
       <c r="F68" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G68" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="D69" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>260</v>
       </c>
       <c r="E69" s="9"/>
       <c r="F69" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G69" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="D70" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>264</v>
       </c>
       <c r="E70" s="9"/>
       <c r="F70" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G70" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G70" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="D71" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>268</v>
       </c>
       <c r="E71" s="9"/>
       <c r="F71" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G71" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="D72" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>272</v>
       </c>
       <c r="E72" s="9"/>
       <c r="F72" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G72" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G72" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="D73" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>276</v>
       </c>
       <c r="E73" s="9"/>
       <c r="F73" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G73" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="D74" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>280</v>
       </c>
       <c r="E74" s="9"/>
       <c r="F74" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G74" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G74" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>283</v>
       </c>
       <c r="E75" s="9"/>
       <c r="F75" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G75" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G75" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>287</v>
       </c>
       <c r="E76" s="9"/>
       <c r="F76" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G76" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G76" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="D77" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>291</v>
       </c>
       <c r="E77" s="9"/>
       <c r="F77" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G77" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G77" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="D78" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>295</v>
       </c>
       <c r="E78" s="9"/>
       <c r="F78" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G78" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G78" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="D79" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>299</v>
       </c>
       <c r="E79" s="9"/>
       <c r="F79" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G79" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G79" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>303</v>
       </c>
       <c r="E80" s="9"/>
       <c r="F80" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G80" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G80" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C81" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>307</v>
       </c>
       <c r="E81" s="9"/>
       <c r="F81" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G81" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G81" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C82" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="F82" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G82" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G82" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="D83" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>315</v>
       </c>
       <c r="E83" s="9"/>
       <c r="F83" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G83" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G83" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="84" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>317</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>319</v>
       </c>
       <c r="E84" s="9"/>
       <c r="F84" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G84" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="G84" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="F85" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D85" s="1" t="s">
+      <c r="G85" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M85" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="G85" s="7" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="M85" s="1" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="F86" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="G86" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="G86" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="E87" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D87" s="1" t="s">
+      <c r="F87" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G87" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="I87" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="E87" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G87" s="7" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="H87" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="I87" s="8" t="s">
-        <v>333</v>
-      </c>
       <c r="K87" s="2" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="L87" s="13" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="F88" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G88" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <v>85</v>
+      </c>
+      <c r="G88" s="7" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>339</v>
-      </c>
       <c r="F89" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G89" s="7" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="G89" s="7" t="s">
+        <v>500</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="M89" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated validation rules; TICC-196
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Participant identifier schemes v8.0.xlsx
+++ b/work-in-progress/Peppol Code Lists - Participant identifier schemes v8.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6260DE6A-A478-46DA-9D87-E49F754550C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08E6812-5C33-4F88-9CDF-6FB53C1B2545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Participant Identifier Scheme" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="504">
   <si>
     <t>Scheme ID</t>
   </si>
@@ -1716,84 +1716,81 @@
     <t>PARTITA IVA</t>
   </si>
   <si>
-    <t>The code is 11 numeric digits
+    <t>FI:ORG</t>
+  </si>
+  <si>
+    <t>0212</t>
+  </si>
+  <si>
+    <t>FI:VAT</t>
+  </si>
+  <si>
+    <t>0213</t>
+  </si>
+  <si>
+    <t>Finnish Organization Identifier</t>
+  </si>
+  <si>
+    <t>State Treasury of Finland / Valtiokonttori</t>
+  </si>
+  <si>
+    <t>9999999-9
+nine characters
+last digit after the hyphen is check character</t>
+  </si>
+  <si>
+    <t>Shall be presented as string so that leading zeros have to be present.
+Hyphen shall be present between last two digits.</t>
+  </si>
+  <si>
+    <t>Character Repertoire: digits 0-9 and hyphen "-"</t>
+  </si>
+  <si>
+    <t>Finnish Organization Value Add Tax Identifier</t>
+  </si>
+  <si>
+    <t>FI99999999
+ten characters</t>
+  </si>
+  <si>
+    <t>Shall be presented as string so that leading zeros have to be present. Two first characters have always fixed value FI.</t>
+  </si>
+  <si>
+    <t>Character Repertoire: digits 0-9 and FI</t>
+  </si>
+  <si>
+    <t>IT:CFI</t>
+  </si>
+  <si>
+    <t>IT:IVA</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>deprecated</t>
+  </si>
+  <si>
+    <t>Deprecation version</t>
+  </si>
+  <si>
+    <t>Up to 46 alphanumeric characters
+Format: &lt;Up to 12 numeric characters&gt;"-"&lt;up to 30 alphanumeric characters&gt;"–"&lt;2 numeric characters&gt;</t>
+  </si>
+  <si>
+    <t>The fine grained part is optional</t>
+  </si>
+  <si>
+    <t>RegEx: [0-9]{2,12}(\-[0-9A-Z]{0,30})?\-[0-9]{2}</t>
+  </si>
+  <si>
+    <t>The code is "IT" followed by 11 numeric digits
 First 7 digits is a progressive number
 The following 3 digits means the province of residence
 The last digit is a check number, calculated using Luhn's Algorithm</t>
-  </si>
-  <si>
-    <t>Character Repertoire: 0 to 9</t>
-  </si>
-  <si>
-    <t>FI:ORG</t>
-  </si>
-  <si>
-    <t>0212</t>
-  </si>
-  <si>
-    <t>FI:VAT</t>
-  </si>
-  <si>
-    <t>0213</t>
-  </si>
-  <si>
-    <t>Finnish Organization Identifier</t>
-  </si>
-  <si>
-    <t>State Treasury of Finland / Valtiokonttori</t>
-  </si>
-  <si>
-    <t>9999999-9
-nine characters
-last digit after the hyphen is check character</t>
-  </si>
-  <si>
-    <t>Shall be presented as string so that leading zeros have to be present.
-Hyphen shall be present between last two digits.</t>
-  </si>
-  <si>
-    <t>Character Repertoire: digits 0-9 and hyphen "-"</t>
-  </si>
-  <si>
-    <t>Finnish Organization Value Add Tax Identifier</t>
-  </si>
-  <si>
-    <t>FI99999999
-ten characters</t>
-  </si>
-  <si>
-    <t>Shall be presented as string so that leading zeros have to be present. Two first characters have always fixed value FI.</t>
-  </si>
-  <si>
-    <t>Character Repertoire: digits 0-9 and FI</t>
-  </si>
-  <si>
-    <t>IT:CFI</t>
-  </si>
-  <si>
-    <t>IT:IVA</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>active</t>
-  </si>
-  <si>
-    <t>deprecated</t>
-  </si>
-  <si>
-    <t>Deprecation version</t>
-  </si>
-  <si>
-    <t>Up to 46 alphanumeric characters
-Format: &lt;Up to 12 numeric characters&gt;"-"&lt;up to 30 alphanumeric characters&gt;"–"&lt;2 numeric characters&gt;</t>
-  </si>
-  <si>
-    <t>The fine grained part is optional</t>
-  </si>
-  <si>
-    <t>RegEx: [0-9]{2,12}(\-[0-9A-Z]{0,30})?\-[0-9]{2}</t>
   </si>
 </sst>
 </file>
@@ -2583,10 +2580,10 @@
   <dimension ref="A1:AMM89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L27" sqref="L27"/>
+      <selection pane="bottomRight" activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2628,10 +2625,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>6</v>
@@ -2669,7 +2666,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>369</v>
@@ -2707,7 +2704,7 @@
         <v>14</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>370</v>
@@ -2742,7 +2739,7 @@
         <v>26</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>371</v>
@@ -2777,7 +2774,7 @@
         <v>14</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>372</v>
@@ -2815,7 +2812,7 @@
         <v>14</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>373</v>
@@ -2853,7 +2850,7 @@
         <v>14</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>49</v>
@@ -2891,7 +2888,7 @@
         <v>14</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>374</v>
@@ -2923,7 +2920,7 @@
         <v>14</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>375</v>
@@ -2958,7 +2955,7 @@
         <v>59</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>376</v>
@@ -2993,7 +2990,7 @@
         <v>64</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>65</v>
@@ -3025,7 +3022,7 @@
         <v>14</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>74</v>
@@ -3057,7 +3054,7 @@
         <v>14</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>128</v>
@@ -3089,7 +3086,7 @@
         <v>80</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>377</v>
@@ -3127,7 +3124,7 @@
         <v>80</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>341</v>
@@ -3162,7 +3159,7 @@
         <v>85</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>378</v>
@@ -3195,7 +3192,7 @@
         <v>90</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I17" s="8" t="s">
         <v>379</v>
@@ -3233,7 +3230,7 @@
         <v>90</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>380</v>
@@ -3271,7 +3268,7 @@
         <v>90</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I19" s="8" t="s">
         <v>101</v>
@@ -3306,7 +3303,7 @@
         <v>107</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>108</v>
@@ -3338,7 +3335,7 @@
         <v>64</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>381</v>
@@ -3373,7 +3370,7 @@
         <v>64</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>382</v>
@@ -3405,7 +3402,7 @@
         <v>80</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>350</v>
@@ -3437,7 +3434,7 @@
         <v>80</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>383</v>
@@ -3469,7 +3466,7 @@
         <v>80</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I25" s="8" t="s">
         <v>124</v>
@@ -3504,7 +3501,7 @@
         <v>361</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I26" s="8" t="s">
         <v>362</v>
@@ -3541,20 +3538,20 @@
         <v>361</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="J27" s="8" t="s">
         <v>368</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="15" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AMM27" s="1"/>
     </row>
@@ -3578,7 +3575,7 @@
         <v>429</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I28" s="8" t="s">
         <v>466</v>
@@ -3612,7 +3609,7 @@
         <v>470</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="8" t="s">
@@ -4645,7 +4642,7 @@
     </row>
     <row r="30" spans="1:1027" ht="255" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>474</v>
@@ -4663,7 +4660,7 @@
         <v>470</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="8" t="s">
@@ -5689,9 +5686,9 @@
       <c r="AML30" s="12"/>
       <c r="AMM30" s="12"/>
     </row>
-    <row r="31" spans="1:1027" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1027" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>475</v>
@@ -5709,15 +5706,15 @@
         <v>470</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="H31" s="12"/>
       <c r="I31" s="8" t="s">
-        <v>481</v>
+        <v>503</v>
       </c>
       <c r="K31" s="15"/>
       <c r="L31" s="13" t="s">
-        <v>482</v>
+        <v>457</v>
       </c>
       <c r="M31" s="12"/>
       <c r="N31" s="12"/>
@@ -6737,36 +6734,36 @@
     </row>
     <row r="32" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F32" s="15" t="s">
         <v>470</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="H32" s="12"/>
       <c r="I32" s="8" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="K32" s="15"/>
       <c r="L32" s="13" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="M32" s="12"/>
       <c r="N32" s="12"/>
@@ -7786,36 +7783,36 @@
     </row>
     <row r="33" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F33" s="15" t="s">
         <v>470</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="H33" s="12"/>
       <c r="I33" s="8" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="K33" s="15"/>
       <c r="L33" s="13" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="M33" s="12"/>
       <c r="N33" s="12"/>
@@ -8853,7 +8850,7 @@
         <v>14</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>128</v>
@@ -8885,7 +8882,7 @@
         <v>14</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="K35" s="2" t="s">
         <v>401</v>
@@ -8914,7 +8911,7 @@
         <v>14</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>135</v>
@@ -8943,7 +8940,7 @@
         <v>14</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>135</v>
@@ -8969,7 +8966,10 @@
         <v>14</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>503</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>142</v>
@@ -8998,7 +8998,7 @@
         <v>14</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>402</v>
@@ -9030,7 +9030,7 @@
         <v>14</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I40" s="8" t="s">
         <v>101</v>
@@ -9062,7 +9062,7 @@
         <v>14</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>151</v>
@@ -9094,7 +9094,7 @@
         <v>14</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="L42" s="13" t="s">
         <v>460</v>
@@ -9118,7 +9118,7 @@
         <v>14</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>151</v>
@@ -9153,7 +9153,7 @@
         <v>14</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="M44" s="1" t="s">
         <v>421</v>
@@ -9176,7 +9176,7 @@
         <v>14</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="K45" s="2" t="s">
         <v>169</v>
@@ -9200,7 +9200,7 @@
         <v>14</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="K46" s="2" t="s">
         <v>403</v>
@@ -9229,7 +9229,7 @@
         <v>14</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>177</v>
@@ -9252,7 +9252,7 @@
         <v>14</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>64</v>
@@ -9290,7 +9290,7 @@
         <v>184</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I49" s="8" t="s">
         <v>384</v>
@@ -9314,7 +9314,7 @@
         <v>177</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I50" s="8" t="s">
         <v>188</v>
@@ -9343,7 +9343,7 @@
         <v>177</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -9366,7 +9366,7 @@
         <v>151</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>361</v>
@@ -9393,7 +9393,7 @@
         <v>151</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -9414,7 +9414,7 @@
         <v>151</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -9435,7 +9435,7 @@
         <v>151</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -9456,7 +9456,7 @@
         <v>151</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -9477,7 +9477,7 @@
         <v>151</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -9498,7 +9498,7 @@
         <v>151</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -9518,7 +9518,7 @@
         <v>151</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
@@ -9539,7 +9539,7 @@
         <v>151</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -9560,7 +9560,7 @@
         <v>151</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -9581,7 +9581,7 @@
         <v>151</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -9602,7 +9602,7 @@
         <v>151</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -9623,7 +9623,7 @@
         <v>151</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -9644,7 +9644,7 @@
         <v>151</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -9665,7 +9665,7 @@
         <v>151</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -9686,7 +9686,7 @@
         <v>151</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -9707,7 +9707,7 @@
         <v>151</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -9728,7 +9728,7 @@
         <v>151</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -9749,7 +9749,7 @@
         <v>151</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -9770,7 +9770,7 @@
         <v>151</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -9791,7 +9791,7 @@
         <v>151</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -9812,7 +9812,7 @@
         <v>151</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -9833,7 +9833,7 @@
         <v>151</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -9854,7 +9854,7 @@
         <v>151</v>
       </c>
       <c r="G75" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -9875,7 +9875,7 @@
         <v>151</v>
       </c>
       <c r="G76" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -9896,7 +9896,7 @@
         <v>151</v>
       </c>
       <c r="G77" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -9917,7 +9917,7 @@
         <v>151</v>
       </c>
       <c r="G78" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -9938,7 +9938,7 @@
         <v>151</v>
       </c>
       <c r="G79" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -9959,7 +9959,7 @@
         <v>151</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
@@ -9980,7 +9980,7 @@
         <v>151</v>
       </c>
       <c r="G81" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -10000,7 +10000,7 @@
         <v>151</v>
       </c>
       <c r="G82" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
@@ -10021,7 +10021,7 @@
         <v>151</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="84" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -10042,7 +10042,7 @@
         <v>151</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
@@ -10062,7 +10062,7 @@
         <v>321</v>
       </c>
       <c r="G85" s="7" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>90</v>
@@ -10088,7 +10088,7 @@
         <v>326</v>
       </c>
       <c r="G86" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="105" x14ac:dyDescent="0.25">
@@ -10111,7 +10111,7 @@
         <v>85</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>465</v>
@@ -10143,7 +10143,7 @@
         <v>85</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
@@ -10163,7 +10163,7 @@
         <v>107</v>
       </c>
       <c r="G89" s="7" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>361</v>

</xml_diff>